<commit_message>
Pushing the code, used Cameron's algorithm to help me, as well as our test cases that we worked on together - Ethan
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameron/PycharmProjects/cs151-sky-ethan_cameron_lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadsouza\PycharmProjects\cs151-sky-ethan_cameron_lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A71D2A9-6149-874D-9B94-90D8591B69FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A5430-7B43-47D3-9A69-44C555484D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Test Description</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Points per Meter</t>
   </si>
   <si>
+    <t>Par (distance)</t>
+  </si>
+  <si>
     <t>Normal</t>
   </si>
   <si>
@@ -105,17 +108,17 @@
     <t>Large Hill, fast speed</t>
   </si>
   <si>
-    <t>large</t>
-  </si>
-  <si>
-    <t>normal</t>
+    <t>Normal Hill</t>
+  </si>
+  <si>
+    <t>Large Hill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +145,12 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -188,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -217,6 +226,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,18 +541,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714008D9-644A-2B47-9D77-29A0AE074340}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -557,7 +569,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -567,7 +579,9 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="1"/>
@@ -576,9 +590,9 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>46</v>
@@ -597,9 +611,9 @@
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>70</v>
@@ -618,7 +632,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -631,7 +645,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -644,19 +658,19 @@
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
@@ -665,48 +679,48 @@
       <c r="J7" s="9"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="46" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1">
         <v>46</v>
@@ -722,22 +736,22 @@
         <v>3.0639443699324591</v>
       </c>
       <c r="H9" s="2">
-        <f>C9*G9</f>
-        <v>61.278887398649182</v>
+        <f>$C$9*$G$9</f>
+        <v>91.918331097973777</v>
       </c>
       <c r="I9" s="2">
-        <f>C9*G9</f>
-        <v>61.278887398649182</v>
+        <f>$C$9*$G$9</f>
+        <v>91.918331097973777</v>
       </c>
       <c r="J9" s="2">
-        <f>60 + (I9 - F9)*E9</f>
-        <v>2.5577747972983644</v>
+        <f>60+(I9-F9)*E9</f>
+        <v>63.836662195947554</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -763,21 +777,21 @@
         <v>275.7549932939213</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I12" si="2">C10*G10</f>
+        <f>C10*G10</f>
         <v>275.7549932939213</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ref="J10:J12" si="3">60 + (I10 - F10)*E10</f>
+        <f t="shared" ref="J10:J13" si="2">60+(I10-F10)*E10</f>
         <v>431.5099865878426</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>30</v>
@@ -800,21 +814,21 @@
         <v>113.38934190276817</v>
       </c>
       <c r="I11" s="2">
+        <f>C11*G11</f>
+        <v>113.38934190276817</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="2"/>
-        <v>113.38934190276817</v>
-      </c>
-      <c r="J11" s="2">
-        <f t="shared" si="3"/>
         <v>48.100815424982699</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1">
         <v>90</v>
@@ -837,14 +851,20 @@
         <v>340.16802570830453</v>
       </c>
       <c r="I12" s="2">
+        <f>C12*G12</f>
+        <v>340.16802570830453</v>
+      </c>
+      <c r="J12" s="2">
         <f t="shared" si="2"/>
-        <v>340.16802570830453</v>
-      </c>
-      <c r="J12" s="2">
-        <f t="shared" si="3"/>
         <v>456.30244627494818</v>
       </c>
       <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -855,5 +875,6 @@
     <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>